<commit_message>
solve issue with tournaments list
</commit_message>
<xml_diff>
--- a/BWF_TOURNAMENTS/2023_BWF_TOURNAMENTS_LIST_WITH_DISTRIBUTION_AND_KEY_DATES_AND_MATCHING.xlsx
+++ b/BWF_TOURNAMENTS/2023_BWF_TOURNAMENTS_LIST_WITH_DISTRIBUTION_AND_KEY_DATES_AND_MATCHING.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\FFBad\Season planner\BWF_TOURNAMENTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BB963D-623C-48BC-8A65-74C976C51401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDCC190-E7E7-4C1F-A82B-AC3923D73F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-80" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2046,7 +2046,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2357,7 +2357,7 @@
   <dimension ref="A1:AF148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>